<commit_message>
analysis all the endpoint
</commit_message>
<xml_diff>
--- a/docs/HuggingfaceAPI.xlsx
+++ b/docs/HuggingfaceAPI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rxhbs7s/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rxhbs7s/projects/transformerz/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1715928-77CB-9C46-B090-646BAC8106A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E73509B-C57F-5443-8C1B-CA302E235751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34560" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{1DD1979F-3FE7-8843-B009-D472AD4E988F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="97">
   <si>
     <t>HF client method</t>
   </si>
@@ -285,13 +285,93 @@
   </si>
   <si>
     <t>Prorities</t>
+  </si>
+  <si>
+    <t>/api/{repo_type}s/{repo_id}/commit/{revision}</t>
+  </si>
+  <si>
+    <t>/api/{repo_type}s/{repo_id}/branch/{branch}</t>
+  </si>
+  <si>
+    <t>/api/{repo_type}s/{repo_id}/tag/{revision}</t>
+  </si>
+  <si>
+    <t>/api/{repo_type}s/{repo_id}/discussions?p={page_index}</t>
+  </si>
+  <si>
+    <t>/api/{repo_type}s/{repo_id}/discussions/{discussion_num}</t>
+  </si>
+  <si>
+    <t>/api/{repo_type}s/{repo_id}/discussions</t>
+  </si>
+  <si>
+    <r>
+      <t>/api/spaces/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>repo_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>/secrets</t>
+    </r>
+  </si>
+  <si>
+    <t>/api/spaces/{repo_id}/secrets</t>
+  </si>
+  <si>
+    <t>/api/spaces/{repo_id}/runtime</t>
+  </si>
+  <si>
+    <t>/api/spaces/{repo_id}/hardware</t>
+  </si>
+  <si>
+    <t>/api/spaces/{repo_id}/sleeptime</t>
+  </si>
+  <si>
+    <t>/api/spaces/{repo_id}/pause</t>
+  </si>
+  <si>
+    <t>/api/spaces/{repo_id}/restart</t>
+  </si>
+  <si>
+    <t>/api/spaces/{from_id}/duplicat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -305,6 +385,24 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6A8759"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC7832"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -348,12 +446,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,7 +767,7 @@
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -954,10 +1050,10 @@
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -1032,7 +1128,9 @@
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="C24" s="1" t="s">
         <v>79</v>
       </c>
@@ -1045,7 +1143,9 @@
       <c r="A25" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="C25" s="1" t="s">
         <v>79</v>
       </c>
@@ -1058,7 +1158,9 @@
       <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="C26" s="1" t="s">
         <v>79</v>
       </c>
@@ -1071,7 +1173,9 @@
       <c r="A27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="C27" s="1" t="s">
         <v>79</v>
       </c>
@@ -1110,7 +1214,9 @@
       <c r="A30" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="1"/>
+      <c r="B30" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="C30" s="1" t="s">
         <v>79</v>
       </c>
@@ -1123,7 +1229,9 @@
       <c r="A31" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B31" s="1"/>
+      <c r="B31" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="C31" s="1" t="s">
         <v>79</v>
       </c>
@@ -1136,7 +1244,9 @@
       <c r="A32" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="C32" s="1" t="s">
         <v>79</v>
       </c>
@@ -1149,7 +1259,9 @@
       <c r="A33" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="1"/>
+      <c r="B33" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="C33" s="1" t="s">
         <v>79</v>
       </c>
@@ -1175,7 +1287,9 @@
       <c r="A35" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="1"/>
+      <c r="B35" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="C35" s="1" t="s">
         <v>78</v>
       </c>
@@ -1188,7 +1302,9 @@
       <c r="A36" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B36" s="1"/>
+      <c r="B36" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="C36" s="1" t="s">
         <v>78</v>
       </c>
@@ -1201,7 +1317,9 @@
       <c r="A37" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="1"/>
+      <c r="B37" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="C37" s="1" t="s">
         <v>78</v>
       </c>
@@ -1214,7 +1332,9 @@
       <c r="A38" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B38" s="1"/>
+      <c r="B38" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="C38" s="1" t="s">
         <v>79</v>
       </c>
@@ -1227,7 +1347,9 @@
       <c r="A39" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="1"/>
+      <c r="B39" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="C39" s="1" t="s">
         <v>78</v>
       </c>
@@ -1240,7 +1362,9 @@
       <c r="A40" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="1"/>
+      <c r="B40" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="C40" s="1" t="s">
         <v>78</v>
       </c>
@@ -1253,7 +1377,9 @@
       <c r="A41" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B41" s="1"/>
+      <c r="B41" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="C41" s="1" t="s">
         <v>78</v>
       </c>
@@ -1266,7 +1392,9 @@
       <c r="A42" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B42" s="1"/>
+      <c r="B42" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="C42" s="1" t="s">
         <v>79</v>
       </c>
@@ -1279,7 +1407,9 @@
       <c r="A43" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B43" s="1"/>
+      <c r="B43" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="C43" s="1" t="s">
         <v>78</v>
       </c>
@@ -1292,7 +1422,9 @@
       <c r="A44" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B44" s="1"/>
+      <c r="B44" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="C44" s="1" t="s">
         <v>78</v>
       </c>
@@ -1301,11 +1433,13 @@
       </c>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B45" s="1"/>
+      <c r="B45" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="C45" s="1" t="s">
         <v>76</v>
       </c>
@@ -1318,7 +1452,9 @@
       <c r="A46" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B46" s="1"/>
+      <c r="B46" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="C46" s="1" t="s">
         <v>76</v>
       </c>
@@ -1331,7 +1467,9 @@
       <c r="A47" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B47" s="1"/>
+      <c r="B47" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="C47" s="1" t="s">
         <v>76</v>
       </c>
@@ -1344,7 +1482,9 @@
       <c r="A48" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B48" s="1"/>
+      <c r="B48" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="C48" s="1" t="s">
         <v>76</v>
       </c>
@@ -1357,7 +1497,9 @@
       <c r="A49" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B49" s="1"/>
+      <c r="B49" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="C49" s="1" t="s">
         <v>76</v>
       </c>
@@ -1370,7 +1512,9 @@
       <c r="A50" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B50" s="1"/>
+      <c r="B50" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="C50" s="1" t="s">
         <v>76</v>
       </c>
@@ -1383,7 +1527,9 @@
       <c r="A51" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B51" s="1"/>
+      <c r="B51" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="C51" s="1" t="s">
         <v>76</v>
       </c>
@@ -1396,7 +1542,9 @@
       <c r="A52" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B52" s="1"/>
+      <c r="B52" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="C52" s="1" t="s">
         <v>76</v>
       </c>
@@ -1404,13 +1552,6 @@
         <v>4</v>
       </c>
       <c r="E52" s="1"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="4"/>
-      <c r="B53" s="4"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">

</xml_diff>